<commit_message>
implemented proper removal of leftovers from the build process; revised README.md
</commit_message>
<xml_diff>
--- a/doc/bugs.xlsx
+++ b/doc/bugs.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="147">
   <si>
     <t>Datum rapporterat</t>
   </si>
@@ -430,9 +430,6 @@
     <t>alpha-3</t>
   </si>
   <si>
-    <t>Fixa en sitemap</t>
-  </si>
-  <si>
     <t>Hur får man in en BTTT-funktionalitet inom samma dokument i index.html?</t>
   </si>
   <si>
@@ -455,6 +452,21 @@
   </si>
   <si>
     <t>Peka ut sajten i LinkedIn</t>
+  </si>
+  <si>
+    <t>Fixa en sitemap. Registrera den hos Google.</t>
+  </si>
+  <si>
+    <t>LinkedIn-badge. Problemet var löst innan jag skrev in det som en bugg, därav de ologiska datumen.</t>
+  </si>
+  <si>
+    <t>alpha-4</t>
+  </si>
+  <si>
+    <t>Varje sida skall ha en h1-rubrik</t>
+  </si>
+  <si>
+    <t>alpha-5</t>
   </si>
 </sst>
 </file>
@@ -923,9 +935,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,7 +979,9 @@
       <c r="B2" s="9">
         <v>43202</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="9">
+        <v>43202</v>
+      </c>
       <c r="D2" s="29" t="s">
         <v>7</v>
       </c>
@@ -975,7 +989,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -992,7 +1006,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1010,7 +1024,7 @@
         <v>7</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1020,7 +1034,9 @@
       <c r="B5" s="9">
         <v>43202</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="12">
+        <v>43203</v>
+      </c>
       <c r="D5" s="29" t="s">
         <v>9</v>
       </c>
@@ -1028,7 +1044,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1046,7 +1062,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1064,12 +1080,12 @@
         <v>8</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="B8" s="9">
         <v>43202</v>
@@ -1079,10 +1095,10 @@
         <v>12</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1092,7 +1108,9 @@
       <c r="B9" s="9">
         <v>43202</v>
       </c>
-      <c r="C9" s="9"/>
+      <c r="C9" s="9">
+        <v>43202</v>
+      </c>
       <c r="D9" s="29" t="s">
         <v>13</v>
       </c>
@@ -1100,12 +1118,12 @@
         <v>7</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="B10" s="9">
         <v>43202</v>
@@ -1114,9 +1132,11 @@
       <c r="D10" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="F10" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1130,7 +1150,12 @@
       <c r="D11" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="30"/>
+      <c r="E11" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="12" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
@@ -1139,12 +1164,18 @@
       <c r="B12" s="9">
         <v>43202</v>
       </c>
-      <c r="C12" s="9"/>
+      <c r="C12" s="9">
+        <v>43201</v>
+      </c>
       <c r="D12" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="18"/>
+      <c r="E12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>143</v>
+      </c>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1161,8 +1192,12 @@
       <c r="E13" s="30"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="9"/>
+      <c r="A14" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" s="9">
+        <v>43202</v>
+      </c>
       <c r="C14" s="9"/>
       <c r="D14" s="29" t="s">
         <v>18</v>
@@ -1171,8 +1206,12 @@
       <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="9"/>
+      <c r="A15" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B15" s="9">
+        <v>43202</v>
+      </c>
       <c r="C15" s="9"/>
       <c r="D15" s="29" t="s">
         <v>19</v>
@@ -1181,8 +1220,12 @@
       <c r="F15" s="21"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="9"/>
+      <c r="A16" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="9">
+        <v>43202</v>
+      </c>
       <c r="C16" s="9"/>
       <c r="D16" s="29" t="s">
         <v>20</v>
@@ -1191,8 +1234,12 @@
       <c r="F16" s="18"/>
     </row>
     <row r="17" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="9"/>
+      <c r="A17" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" s="9">
+        <v>43202</v>
+      </c>
       <c r="C17" s="12"/>
       <c r="D17" s="29" t="s">
         <v>21</v>
@@ -1201,8 +1248,12 @@
       <c r="F17" s="20"/>
     </row>
     <row r="18" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="10"/>
+      <c r="A18" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B18" s="9">
+        <v>43202</v>
+      </c>
       <c r="C18" s="10"/>
       <c r="D18" s="29" t="s">
         <v>22</v>
@@ -1211,7 +1262,12 @@
       <c r="F18" s="18"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
+      <c r="A19" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B19" s="9">
+        <v>43202</v>
+      </c>
       <c r="C19" s="9"/>
       <c r="D19" s="29" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
added Google Analytics code
</commit_message>
<xml_diff>
--- a/doc/bugs.xlsx
+++ b/doc/bugs.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="148">
   <si>
     <t>Datum rapporterat</t>
   </si>
@@ -467,6 +467,10 @@
   </si>
   <si>
     <t>alpha-5</t>
+  </si>
+  <si>
+    <t>Ställ in user-ID för Google Analytics: 
+https://analytics.google.com/analytics/web/?authuser=0#/a60939522w95510629p99580428/admin/tracking/user-id/</t>
   </si>
 </sst>
 </file>
@@ -937,7 +941,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,9 +1182,9 @@
       </c>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="B13" s="9">
         <v>43202</v>
@@ -1189,7 +1193,12 @@
       <c r="D13" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="30"/>
+      <c r="E13" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">

</xml_diff>

<commit_message>
added proper language code to all html pages; added a meta-description to all html pages
</commit_message>
<xml_diff>
--- a/doc/bugs.xlsx
+++ b/doc/bugs.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="149">
   <si>
     <t>Datum rapporterat</t>
   </si>
@@ -471,6 +471,10 @@
   <si>
     <t>Ställ in user-ID för Google Analytics: 
 https://analytics.google.com/analytics/web/?authuser=0#/a60939522w95510629p99580428/admin/tracking/user-id/</t>
+  </si>
+  <si>
+    <t>&lt;meta name="author" content="Thomas J. Ekman"&gt;
+&lt;html lang="sv"&gt;</t>
   </si>
 </sst>
 </file>
@@ -939,9 +943,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1200,19 +1204,21 @@
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>133</v>
       </c>
       <c r="B14" s="9">
-        <v>43202</v>
+        <v>43203</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="29" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="31"/>
-      <c r="F14" s="21"/>
+      <c r="F14" s="21" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">

</xml_diff>

<commit_message>
added meta tag for author
</commit_message>
<xml_diff>
--- a/doc/bugs.xlsx
+++ b/doc/bugs.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="151">
   <si>
     <t>Datum rapporterat</t>
   </si>
@@ -473,8 +473,13 @@
 https://analytics.google.com/analytics/web/?authuser=0#/a60939522w95510629p99580428/admin/tracking/user-id/</t>
   </si>
   <si>
-    <t>&lt;meta name="author" content="Thomas J. Ekman"&gt;
-&lt;html lang="sv"&gt;</t>
+    <t>&lt;html lang="sv"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;meta name="author" content="Thomas J. Ekman"&gt;</t>
+  </si>
+  <si>
+    <t>meta-taggen för copyright</t>
   </si>
 </sst>
 </file>
@@ -945,7 +950,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,14 +1209,16 @@
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>133</v>
       </c>
       <c r="B14" s="9">
         <v>43203</v>
       </c>
-      <c r="C14" s="9"/>
+      <c r="C14" s="9">
+        <v>43203</v>
+      </c>
       <c r="D14" s="29" t="s">
         <v>18</v>
       </c>
@@ -1227,12 +1234,16 @@
       <c r="B15" s="9">
         <v>43202</v>
       </c>
-      <c r="C15" s="9"/>
+      <c r="C15" s="9">
+        <v>43203</v>
+      </c>
       <c r="D15" s="29" t="s">
         <v>19</v>
       </c>
       <c r="E15" s="7"/>
-      <c r="F15" s="21"/>
+      <c r="F15" s="21" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
@@ -1246,7 +1257,9 @@
         <v>20</v>
       </c>
       <c r="E16" s="7"/>
-      <c r="F16" s="18"/>
+      <c r="F16" s="18" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="17" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">

</xml_diff>

<commit_message>
changed build settings for the two images displaying my university degree
</commit_message>
<xml_diff>
--- a/doc/bugs.xlsx
+++ b/doc/bugs.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="152">
   <si>
     <t>Datum rapporterat</t>
   </si>
@@ -480,6 +480,9 @@
   </si>
   <si>
     <t>meta-taggen för copyright</t>
+  </si>
+  <si>
+    <t>directories img och css blir kvar när man gör en cleanup</t>
   </si>
 </sst>
 </file>
@@ -950,7 +953,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,14 +1269,16 @@
         <v>133</v>
       </c>
       <c r="B17" s="9">
-        <v>43202</v>
+        <v>43203</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="29" t="s">
         <v>21</v>
       </c>
       <c r="E17" s="30"/>
-      <c r="F17" s="20"/>
+      <c r="F17" s="20" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="18" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">

</xml_diff>

<commit_message>
changed header level on pages, so that each have at least one h1 header level
</commit_message>
<xml_diff>
--- a/doc/bugs.xlsx
+++ b/doc/bugs.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="151">
   <si>
     <t>Datum rapporterat</t>
   </si>
@@ -442,9 +442,6 @@
     <t>SEO - ongoing process</t>
   </si>
   <si>
-    <t>Komplettera &lt;head&gt;-sektionen med author och copyright, även om det inte är någon / något som läser denna information</t>
-  </si>
-  <si>
     <t>Lös problemet med att rubrikerna syns i index.html när man surfar in på sidan</t>
   </si>
   <si>
@@ -464,9 +461,6 @@
   </si>
   <si>
     <t>Varje sida skall ha en h1-rubrik</t>
-  </si>
-  <si>
-    <t>alpha-5</t>
   </si>
   <si>
     <t>Ställ in user-ID för Google Analytics: 
@@ -482,14 +476,18 @@
     <t>meta-taggen för copyright</t>
   </si>
   <si>
-    <t>directories img och css blir kvar när man gör en cleanup</t>
+    <t>directories img och css blir kvar när man gör en cleanup. (Det skall de göra, eftersom cleanup.cmd anropas som en del av post-build step).</t>
+  </si>
+  <si>
+    <t>Komplettera &lt;head&gt;-sektionen med author och copyright, även om det inte är någon / något som läser denna information
+(Duplikat av ID 14-15)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -526,6 +524,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -553,7 +558,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -648,6 +653,19 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -949,11 +967,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G128"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,7 +1007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>133</v>
       </c>
@@ -1005,12 +1024,12 @@
         <v>7</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="B3" s="9">
         <v>43202</v>
@@ -1019,7 +1038,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>134</v>
@@ -1043,7 +1062,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>133</v>
       </c>
@@ -1081,27 +1100,29 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="11">
         <v>43202</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="29" t="s">
+      <c r="C7" s="35">
+        <v>43203</v>
+      </c>
+      <c r="D7" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="21" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7" s="37" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B8" s="9">
         <v>43202</v>
@@ -1114,10 +1135,10 @@
         <v>7</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>133</v>
       </c>
@@ -1134,12 +1155,12 @@
         <v>7</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B10" s="9">
         <v>43202</v>
@@ -1152,17 +1173,19 @@
         <v>6</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>133</v>
       </c>
       <c r="B11" s="9">
         <v>43202</v>
       </c>
-      <c r="C11" s="9"/>
+      <c r="C11" s="9">
+        <v>43203</v>
+      </c>
       <c r="D11" s="29" t="s">
         <v>15</v>
       </c>
@@ -1170,10 +1193,10 @@
         <v>6</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>133</v>
       </c>
@@ -1190,13 +1213,13 @@
         <v>7</v>
       </c>
       <c r="F12" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
         <v>143</v>
-      </c>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>144</v>
       </c>
       <c r="B13" s="9">
         <v>43202</v>
@@ -1209,10 +1232,10 @@
         <v>6</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>133</v>
       </c>
@@ -1225,12 +1248,14 @@
       <c r="D14" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="31"/>
+      <c r="E14" s="31" t="s">
+        <v>6</v>
+      </c>
       <c r="F14" s="21" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>133</v>
       </c>
@@ -1243,14 +1268,16 @@
       <c r="D15" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="F15" s="21" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="B16" s="9">
         <v>43202</v>
@@ -1259,25 +1286,29 @@
       <c r="D16" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="7"/>
+      <c r="E16" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="F16" s="18" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="11">
         <v>43203</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="29" t="s">
+      <c r="C17" s="11">
+        <v>43203</v>
+      </c>
+      <c r="D17" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="30"/>
-      <c r="F17" s="20" t="s">
-        <v>151</v>
+      <c r="E17" s="27"/>
+      <c r="F17" s="19" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1307,7 +1338,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="C20" s="9"/>
       <c r="D20" s="29" t="s">
@@ -1315,7 +1346,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
       <c r="B21" s="11"/>
       <c r="C21" s="9"/>
@@ -1325,7 +1356,7 @@
       <c r="E21" s="27"/>
       <c r="F21" s="19"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="C22" s="9"/>
       <c r="D22" s="29" t="s">
@@ -1334,7 +1365,7 @@
       <c r="E22" s="7"/>
       <c r="F22" s="18"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -1344,20 +1375,20 @@
       <c r="E23" s="7"/>
       <c r="F23" s="18"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="C24" s="12"/>
       <c r="D24" s="29" t="s">
         <v>28</v>
       </c>
       <c r="E24" s="30"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D25" s="29" t="s">
         <v>29</v>
       </c>
       <c r="E25" s="30"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
@@ -1367,35 +1398,35 @@
       <c r="E26" s="31"/>
       <c r="F26" s="21"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="D27" s="29" t="s">
         <v>31</v>
       </c>
       <c r="E27" s="30"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="D28" s="29" t="s">
         <v>32</v>
       </c>
       <c r="E28" s="30"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="D29" s="29" t="s">
         <v>33</v>
       </c>
       <c r="E29" s="30"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="D30" s="29" t="s">
         <v>34</v>
       </c>
       <c r="E30" s="30"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -1405,13 +1436,13 @@
       <c r="E31" s="27"/>
       <c r="F31" s="19"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D32" s="29" t="s">
         <v>36</v>
       </c>
       <c r="E32" s="30"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="28"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
@@ -1421,13 +1452,13 @@
       <c r="E33" s="31"/>
       <c r="F33" s="21"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D34" s="29" t="s">
         <v>38</v>
       </c>
       <c r="E34" s="30"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14"/>
       <c r="C35" s="9"/>
       <c r="D35" s="29" t="s">
@@ -1435,21 +1466,21 @@
       </c>
       <c r="E35" s="30"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="C36" s="9"/>
       <c r="D36" s="29" t="s">
         <v>40</v>
       </c>
       <c r="E36" s="30"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="C37" s="9"/>
       <c r="D37" s="29" t="s">
         <v>41</v>
       </c>
       <c r="E37" s="30"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
       <c r="C38" s="9"/>
       <c r="D38" s="29" t="s">
@@ -1457,21 +1488,21 @@
       </c>
       <c r="E38" s="30"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="C39" s="9"/>
       <c r="D39" s="29" t="s">
         <v>43</v>
       </c>
       <c r="E39" s="30"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="C40" s="9"/>
       <c r="D40" s="29" t="s">
         <v>44</v>
       </c>
       <c r="E40" s="30"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="14"/>
       <c r="C41" s="9"/>
       <c r="D41" s="29" t="s">
@@ -1479,7 +1510,7 @@
       </c>
       <c r="E41" s="30"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
       <c r="D42" s="29" t="s">
@@ -1488,7 +1519,7 @@
       <c r="E42" s="27"/>
       <c r="F42" s="19"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -1498,7 +1529,7 @@
       <c r="E43" s="27"/>
       <c r="F43" s="19"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -1508,7 +1539,7 @@
       <c r="E44" s="27"/>
       <c r="F44" s="19"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -1518,14 +1549,14 @@
       <c r="E45" s="27"/>
       <c r="F45" s="19"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="14"/>
       <c r="D46" s="29" t="s">
         <v>50</v>
       </c>
       <c r="E46" s="30"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14"/>
       <c r="C47" s="9"/>
       <c r="D47" s="29" t="s">
@@ -1533,7 +1564,7 @@
       </c>
       <c r="E47" s="30"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="14"/>
       <c r="C48" s="9"/>
       <c r="D48" s="29" t="s">
@@ -1541,7 +1572,7 @@
       </c>
       <c r="E48" s="30"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14"/>
       <c r="C49" s="9"/>
       <c r="D49" s="29" t="s">
@@ -1549,92 +1580,92 @@
       </c>
       <c r="E49" s="30"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D50" s="29" t="s">
         <v>54</v>
       </c>
       <c r="E50" s="30"/>
       <c r="F50" s="22"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D51" s="29" t="s">
         <v>55</v>
       </c>
       <c r="E51" s="30"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D52" s="29" t="s">
         <v>56</v>
       </c>
       <c r="E52" s="30"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D53" s="29" t="s">
         <v>57</v>
       </c>
       <c r="E53" s="30"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="C54" s="9"/>
       <c r="D54" s="29" t="s">
         <v>58</v>
       </c>
       <c r="E54" s="30"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D55" s="29" t="s">
         <v>59</v>
       </c>
       <c r="E55" s="30"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D56" s="29" t="s">
         <v>60</v>
       </c>
       <c r="E56" s="30"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="C57" s="9"/>
       <c r="D57" s="29" t="s">
         <v>61</v>
       </c>
       <c r="E57" s="30"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="14"/>
       <c r="D58" s="29" t="s">
         <v>62</v>
       </c>
       <c r="E58" s="30"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D59" s="29" t="s">
         <v>63</v>
       </c>
       <c r="E59" s="30"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="14"/>
       <c r="D60" s="29" t="s">
         <v>64</v>
       </c>
       <c r="E60" s="30"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="14"/>
       <c r="D61" s="29" t="s">
         <v>65</v>
       </c>
       <c r="E61" s="30"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="14"/>
       <c r="D62" s="29" t="s">
         <v>66</v>
       </c>
       <c r="E62" s="30"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="14"/>
       <c r="B63" s="12"/>
       <c r="C63" s="12"/>
@@ -1644,38 +1675,38 @@
       <c r="E63" s="31"/>
       <c r="F63" s="21"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="14"/>
       <c r="D64" s="29" t="s">
         <v>68</v>
       </c>
       <c r="E64" s="30"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D65" s="29" t="s">
         <v>69</v>
       </c>
       <c r="E65" s="30"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D66" s="29" t="s">
         <v>70</v>
       </c>
       <c r="E66" s="30"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D67" s="29" t="s">
         <v>71</v>
       </c>
       <c r="E67" s="30"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D68" s="29" t="s">
         <v>72</v>
       </c>
       <c r="E68" s="30"/>
     </row>
-    <row r="69" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="14"/>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
@@ -1685,7 +1716,7 @@
       <c r="E69" s="7"/>
       <c r="F69" s="18"/>
     </row>
-    <row r="70" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="16"/>
       <c r="B70" s="11"/>
       <c r="C70" s="11"/>
@@ -1695,7 +1726,7 @@
       <c r="E70" s="27"/>
       <c r="F70" s="19"/>
     </row>
-    <row r="71" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="28"/>
       <c r="B71" s="12"/>
       <c r="C71" s="12"/>
@@ -1705,7 +1736,7 @@
       <c r="E71" s="31"/>
       <c r="F71" s="21"/>
     </row>
-    <row r="72" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="15"/>
       <c r="B72" s="10"/>
       <c r="C72" s="33"/>
@@ -1715,7 +1746,7 @@
       <c r="E72" s="30"/>
       <c r="F72" s="20"/>
     </row>
-    <row r="73" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="15"/>
       <c r="B73" s="10"/>
       <c r="C73" s="10"/>
@@ -1725,7 +1756,7 @@
       <c r="E73" s="30"/>
       <c r="F73" s="20"/>
     </row>
-    <row r="74" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="15"/>
       <c r="B74" s="10"/>
       <c r="C74" s="10"/>
@@ -1735,7 +1766,7 @@
       <c r="E74" s="30"/>
       <c r="F74" s="22"/>
     </row>
-    <row r="75" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="15"/>
       <c r="B75" s="10"/>
       <c r="C75" s="10"/>
@@ -1745,13 +1776,13 @@
       <c r="E75" s="30"/>
       <c r="F75" s="20"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D76" s="29" t="s">
         <v>80</v>
       </c>
       <c r="E76" s="30"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="16"/>
       <c r="B77" s="11"/>
       <c r="C77" s="11"/>
@@ -1761,130 +1792,130 @@
       <c r="E77" s="27"/>
       <c r="F77" s="19"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D78" s="29" t="s">
         <v>82</v>
       </c>
       <c r="E78" s="30"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D79" s="29" t="s">
         <v>83</v>
       </c>
       <c r="E79" s="30"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D80" s="29" t="s">
         <v>84</v>
       </c>
       <c r="E80" s="30"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D81" s="29" t="s">
         <v>85</v>
       </c>
       <c r="E81" s="30"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D82" s="29" t="s">
         <v>86</v>
       </c>
       <c r="E82" s="30"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D83" s="29" t="s">
         <v>87</v>
       </c>
       <c r="E83" s="30"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D84" s="29" t="s">
         <v>88</v>
       </c>
       <c r="E84" s="30"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D85" s="29" t="s">
         <v>89</v>
       </c>
       <c r="E85" s="30"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D86" s="29" t="s">
         <v>90</v>
       </c>
       <c r="E86" s="30"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D87" s="29" t="s">
         <v>91</v>
       </c>
       <c r="E87" s="30"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D88" s="29" t="s">
         <v>92</v>
       </c>
       <c r="E88" s="30"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D89" s="29" t="s">
         <v>93</v>
       </c>
       <c r="E89" s="30"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D90" s="29" t="s">
         <v>94</v>
       </c>
       <c r="E90" s="30"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D91" s="29" t="s">
         <v>95</v>
       </c>
       <c r="E91" s="30"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D92" s="29" t="s">
         <v>96</v>
       </c>
       <c r="E92" s="30"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D93" s="29" t="s">
         <v>97</v>
       </c>
       <c r="E93" s="30"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="14"/>
       <c r="D94" s="29" t="s">
         <v>98</v>
       </c>
       <c r="E94" s="30"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="D95" s="29" t="s">
         <v>99</v>
       </c>
       <c r="E95" s="30"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="14"/>
       <c r="D96" s="29" t="s">
         <v>100</v>
       </c>
       <c r="E96" s="30"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="14"/>
       <c r="D97" s="29" t="s">
         <v>101</v>
       </c>
       <c r="E97" s="30"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="16"/>
       <c r="B98" s="11"/>
       <c r="C98" s="11"/>
@@ -1894,7 +1925,7 @@
       <c r="E98" s="27"/>
       <c r="F98" s="19"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="16"/>
       <c r="B99" s="11"/>
       <c r="C99" s="11"/>
@@ -1904,19 +1935,19 @@
       <c r="E99" s="27"/>
       <c r="F99" s="19"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D100" s="29" t="s">
         <v>104</v>
       </c>
       <c r="E100" s="32"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D101" s="29" t="s">
         <v>105</v>
       </c>
       <c r="E101" s="32"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="28"/>
       <c r="B102" s="12"/>
       <c r="C102" s="12"/>
@@ -1926,70 +1957,70 @@
       <c r="E102" s="31"/>
       <c r="F102" s="21"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D103" s="29" t="s">
         <v>107</v>
       </c>
       <c r="E103" s="30"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D104" s="29" t="s">
         <v>108</v>
       </c>
       <c r="E104" s="30"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D105" s="29" t="s">
         <v>109</v>
       </c>
       <c r="E105" s="32"/>
       <c r="F105" s="22"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D106" s="29" t="s">
         <v>110</v>
       </c>
       <c r="E106" s="30"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D107" s="29" t="s">
         <v>111</v>
       </c>
       <c r="E107" s="32"/>
       <c r="F107" s="22"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D108" s="29" t="s">
         <v>112</v>
       </c>
       <c r="E108" s="30"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D109" s="29" t="s">
         <v>113</v>
       </c>
       <c r="E109" s="30"/>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D110" s="29" t="s">
         <v>114</v>
       </c>
       <c r="E110" s="30"/>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D111" s="29" t="s">
         <v>115</v>
       </c>
       <c r="E111" s="30"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="D112" s="29" t="s">
         <v>116</v>
       </c>
       <c r="E112" s="30"/>
       <c r="G112" s="22"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="23"/>
       <c r="B113" s="24"/>
       <c r="C113" s="24"/>
@@ -1999,19 +2030,19 @@
       <c r="E113" s="32"/>
       <c r="F113" s="22"/>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D114" s="29" t="s">
         <v>118</v>
       </c>
       <c r="E114" s="30"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D115" s="29" t="s">
         <v>119</v>
       </c>
       <c r="E115" s="30"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="16"/>
       <c r="B116" s="11"/>
       <c r="C116" s="11"/>
@@ -2021,80 +2052,163 @@
       <c r="E116" s="27"/>
       <c r="F116" s="19"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D117" s="29" t="s">
         <v>121</v>
       </c>
       <c r="E117" s="30"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D118" s="29" t="s">
         <v>122</v>
       </c>
       <c r="E118" s="30"/>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D119" s="29" t="s">
         <v>123</v>
       </c>
       <c r="E119" s="30"/>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D120" s="29" t="s">
         <v>124</v>
       </c>
       <c r="E120" s="30"/>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D121" s="29" t="s">
         <v>125</v>
       </c>
       <c r="E121" s="30"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D122" s="29" t="s">
         <v>126</v>
       </c>
       <c r="E122" s="30"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D123" s="29" t="s">
         <v>127</v>
       </c>
       <c r="E123" s="32"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D124" s="29" t="s">
         <v>128</v>
       </c>
       <c r="E124" s="30"/>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D125" s="29" t="s">
         <v>129</v>
       </c>
       <c r="E125" s="30"/>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D126" s="29" t="s">
         <v>130</v>
       </c>
       <c r="E126" s="30"/>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D127" s="29" t="s">
         <v>131</v>
       </c>
       <c r="E127" s="30"/>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D128" s="29" t="s">
         <v>132</v>
       </c>
       <c r="E128" s="30"/>
     </row>
+    <row r="129" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="130" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="131" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="132" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="133" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="134" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="135" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="136" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="137" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="138" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="139" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="140" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="141" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="142" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="143" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="144" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="145" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="146" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="147" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="148" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="149" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="150" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="151" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="152" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="153" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="154" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="155" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="156" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="157" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="158" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="159" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="160" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="161" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="162" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="163" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="164" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="165" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="166" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="167" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="168" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="169" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="170" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="171" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="172" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="173" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="174" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="175" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="176" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="177" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="178" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="179" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="180" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="181" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="182" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="183" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="184" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="185" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="186" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="187" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="188" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="189" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="190" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="191" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="192" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="193" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="194" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="195" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="196" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="197" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="198" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="199" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="200" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="201" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="202" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:G202"/>
+  <autoFilter ref="A1:G202">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="alpha-3"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
replaced container-fluid by container; widened central text from 6 to 8 blocks; added text block directly under h1 in personal.html; added text block directly under h2 for "Databaser" header in techniques.html; revised bug tracking document;
</commit_message>
<xml_diff>
--- a/doc/bugs.xlsx
+++ b/doc/bugs.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="162">
   <si>
     <t>Datum rapporterat</t>
   </si>
@@ -433,15 +433,9 @@
     <t>Hur får man in en BTTT-funktionalitet inom samma dokument i index.html?</t>
   </si>
   <si>
-    <t>Google Analytics</t>
-  </si>
-  <si>
     <t>Någon form av byggmekanism så att endast de filer som är relevanta för hemsidan kopieras till en deploymentkatalog</t>
   </si>
   <si>
-    <t>SEO - ongoing process</t>
-  </si>
-  <si>
     <t>Lös problemet med att rubrikerna syns i index.html när man surfar in på sidan</t>
   </si>
   <si>
@@ -463,17 +457,10 @@
     <t>Varje sida skall ha en h1-rubrik</t>
   </si>
   <si>
-    <t>Ställ in user-ID för Google Analytics: 
-https://analytics.google.com/analytics/web/?authuser=0#/a60939522w95510629p99580428/admin/tracking/user-id/</t>
-  </si>
-  <si>
     <t>&lt;html lang="sv"&gt;</t>
   </si>
   <si>
     <t>&lt;meta name="author" content="Thomas J. Ekman"&gt;</t>
-  </si>
-  <si>
-    <t>meta-taggen för copyright</t>
   </si>
   <si>
     <t>directories img och css blir kvar när man gör en cleanup. (Det skall de göra, eftersom cleanup.cmd anropas som en del av post-build step).</t>
@@ -481,6 +468,75 @@
   <si>
     <t>Komplettera &lt;head&gt;-sektionen med author och copyright, även om det inte är någon / något som läser denna information
 (Duplikat av ID 14-15)</t>
+  </si>
+  <si>
+    <t>Revidera texten i meta description så att den blir lite fylligare</t>
+  </si>
+  <si>
+    <t>Google Analytics. Kommer att stå som en ständig punkt.</t>
+  </si>
+  <si>
+    <t>SEO - kommer att stå som en ständig punkt.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">meta-taggen för copyright. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Utgår</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Jag har ingen produkt som behöver varumärkesskyddas.</t>
+    </r>
+  </si>
+  <si>
+    <t>Menyn måste centreras.</t>
+  </si>
+  <si>
+    <t>Ställ in user-ID för Google Analytics: 
+https://analytics.google.com/analytics/web/?authuser=0#/a60939522w95510629p99580428/admin/tracking/user-id/
+Kod för Google Analytics implementerad på annat, nytt sätt.</t>
+  </si>
+  <si>
+    <t>Varje sida skall ha åtminstone en h2-rubrik</t>
+  </si>
+  <si>
+    <t>Kolla om det är flera meta-taggar som behövs. Sajten heter www.metatags.org.</t>
+  </si>
+  <si>
+    <t>Lägg till musiklyssning och fotografering som personliga intressen.</t>
+  </si>
+  <si>
+    <t>Byt bakgrundsmönster till något trevligare, mer levande.</t>
+  </si>
+  <si>
+    <t>Porträttbilden - försök få en rund inramning. Jag har sett det någonstans på www.w3schools.com.</t>
+  </si>
+  <si>
+    <t>Klick på mitt porträtt är en mailto-länk</t>
+  </si>
+  <si>
+    <t>Bättre lösning vid bygget. Översyn cleanup.cmd - gör ett post build-step som kopierar filerna till d:\temp\Deploy Homepage\deploy. Då kan man göra deltree på deploy före bygget.</t>
+  </si>
+  <si>
+    <t>Nu skall SEO-arbetet påbörjas på riktigt.</t>
+  </si>
+  <si>
+    <t>Går det att få till en högersida i Google som visar bara kontaktinformationen?</t>
   </si>
 </sst>
 </file>
@@ -968,11 +1024,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G202"/>
+  <dimension ref="A1:G128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,12 +1080,12 @@
         <v>7</v>
       </c>
       <c r="F2" s="18" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>143</v>
       </c>
       <c r="B3" s="9">
         <v>43202</v>
@@ -1044,7 +1100,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>133</v>
       </c>
@@ -1059,7 +1115,7 @@
         <v>7</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1079,10 +1135,10 @@
         <v>6</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>133</v>
       </c>
@@ -1097,7 +1153,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1117,12 +1173,12 @@
         <v>8</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B8" s="9">
         <v>43202</v>
@@ -1135,7 +1191,7 @@
         <v>7</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1155,12 +1211,12 @@
         <v>7</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B10" s="9">
         <v>43202</v>
@@ -1173,7 +1229,7 @@
         <v>6</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1193,7 +1249,7 @@
         <v>6</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -1213,18 +1269,20 @@
         <v>7</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B13" s="9">
         <v>43202</v>
       </c>
-      <c r="C13" s="9"/>
+      <c r="C13" s="10">
+        <v>43205</v>
+      </c>
       <c r="D13" s="29" t="s">
         <v>17</v>
       </c>
@@ -1232,7 +1290,7 @@
         <v>6</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1252,7 +1310,7 @@
         <v>6</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1272,17 +1330,19 @@
         <v>8</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B16" s="9">
         <v>43202</v>
       </c>
-      <c r="C16" s="9"/>
+      <c r="C16" s="10">
+        <v>43205</v>
+      </c>
       <c r="D16" s="29" t="s">
         <v>20</v>
       </c>
@@ -1290,7 +1350,7 @@
         <v>8</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -1306,127 +1366,225 @@
       <c r="D17" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="27"/>
+      <c r="E17" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="F17" s="19" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>133</v>
       </c>
       <c r="B18" s="9">
-        <v>43202</v>
-      </c>
-      <c r="C18" s="10"/>
+        <v>43203</v>
+      </c>
+      <c r="C18" s="10">
+        <v>43205</v>
+      </c>
       <c r="D18" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="18"/>
+      <c r="E18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B19" s="9">
-        <v>43202</v>
+        <v>43205</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="7"/>
+      <c r="E19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="C20" s="9"/>
+      <c r="A20" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" s="10">
+        <v>43205</v>
+      </c>
+      <c r="C20" s="10">
+        <v>43205</v>
+      </c>
       <c r="D20" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-      <c r="B21" s="11"/>
+      <c r="E20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B21" s="9">
+        <v>43205</v>
+      </c>
       <c r="C21" s="9"/>
       <c r="D21" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="27"/>
-      <c r="F21" s="19"/>
-    </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+      <c r="E21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22" s="9">
+        <v>43205</v>
+      </c>
       <c r="C22" s="9"/>
       <c r="D22" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="18"/>
-    </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="9"/>
+      <c r="E22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="9">
+        <v>43205</v>
+      </c>
       <c r="C23" s="9"/>
       <c r="D23" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="18"/>
-    </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" s="9">
+        <v>43205</v>
+      </c>
       <c r="C24" s="12"/>
       <c r="D24" s="29" t="s">
         <v>28</v>
       </c>
       <c r="E24" s="30"/>
-    </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B25" s="9">
+        <v>43205</v>
+      </c>
       <c r="D25" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="E25" s="30"/>
-    </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="12"/>
+      <c r="E25" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26" s="9">
+        <v>43205</v>
+      </c>
       <c r="C26" s="12"/>
       <c r="D26" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="31"/>
-      <c r="F26" s="21"/>
-    </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
+      <c r="E26" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B27" s="9">
+        <v>43205</v>
+      </c>
       <c r="D27" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E27" s="30"/>
-    </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
+      <c r="E27" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" s="9">
+        <v>43205</v>
+      </c>
       <c r="D28" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="30"/>
-    </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E28" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="D29" s="29" t="s">
         <v>33</v>
       </c>
       <c r="E29" s="30"/>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="D30" s="29" t="s">
         <v>34</v>
       </c>
       <c r="E30" s="30"/>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -1436,13 +1594,13 @@
       <c r="E31" s="27"/>
       <c r="F31" s="19"/>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D32" s="29" t="s">
         <v>36</v>
       </c>
       <c r="E32" s="30"/>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="28"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
@@ -1452,13 +1610,13 @@
       <c r="E33" s="31"/>
       <c r="F33" s="21"/>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D34" s="29" t="s">
         <v>38</v>
       </c>
       <c r="E34" s="30"/>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="14"/>
       <c r="C35" s="9"/>
       <c r="D35" s="29" t="s">
@@ -1466,21 +1624,21 @@
       </c>
       <c r="E35" s="30"/>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C36" s="9"/>
       <c r="D36" s="29" t="s">
         <v>40</v>
       </c>
       <c r="E36" s="30"/>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C37" s="9"/>
       <c r="D37" s="29" t="s">
         <v>41</v>
       </c>
       <c r="E37" s="30"/>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
       <c r="C38" s="9"/>
       <c r="D38" s="29" t="s">
@@ -1488,21 +1646,21 @@
       </c>
       <c r="E38" s="30"/>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C39" s="9"/>
       <c r="D39" s="29" t="s">
         <v>43</v>
       </c>
       <c r="E39" s="30"/>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C40" s="9"/>
       <c r="D40" s="29" t="s">
         <v>44</v>
       </c>
       <c r="E40" s="30"/>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="14"/>
       <c r="C41" s="9"/>
       <c r="D41" s="29" t="s">
@@ -1510,7 +1668,7 @@
       </c>
       <c r="E41" s="30"/>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
       <c r="D42" s="29" t="s">
@@ -1519,7 +1677,7 @@
       <c r="E42" s="27"/>
       <c r="F42" s="19"/>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="16"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -1529,7 +1687,7 @@
       <c r="E43" s="27"/>
       <c r="F43" s="19"/>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -1539,7 +1697,7 @@
       <c r="E44" s="27"/>
       <c r="F44" s="19"/>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="16"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -1549,14 +1707,14 @@
       <c r="E45" s="27"/>
       <c r="F45" s="19"/>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="14"/>
       <c r="D46" s="29" t="s">
         <v>50</v>
       </c>
       <c r="E46" s="30"/>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="14"/>
       <c r="C47" s="9"/>
       <c r="D47" s="29" t="s">
@@ -1564,7 +1722,7 @@
       </c>
       <c r="E47" s="30"/>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="14"/>
       <c r="C48" s="9"/>
       <c r="D48" s="29" t="s">
@@ -1572,7 +1730,7 @@
       </c>
       <c r="E48" s="30"/>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="14"/>
       <c r="C49" s="9"/>
       <c r="D49" s="29" t="s">
@@ -1580,92 +1738,92 @@
       </c>
       <c r="E49" s="30"/>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D50" s="29" t="s">
         <v>54</v>
       </c>
       <c r="E50" s="30"/>
       <c r="F50" s="22"/>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D51" s="29" t="s">
         <v>55</v>
       </c>
       <c r="E51" s="30"/>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D52" s="29" t="s">
         <v>56</v>
       </c>
       <c r="E52" s="30"/>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D53" s="29" t="s">
         <v>57</v>
       </c>
       <c r="E53" s="30"/>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C54" s="9"/>
       <c r="D54" s="29" t="s">
         <v>58</v>
       </c>
       <c r="E54" s="30"/>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D55" s="29" t="s">
         <v>59</v>
       </c>
       <c r="E55" s="30"/>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D56" s="29" t="s">
         <v>60</v>
       </c>
       <c r="E56" s="30"/>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C57" s="9"/>
       <c r="D57" s="29" t="s">
         <v>61</v>
       </c>
       <c r="E57" s="30"/>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="14"/>
       <c r="D58" s="29" t="s">
         <v>62</v>
       </c>
       <c r="E58" s="30"/>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D59" s="29" t="s">
         <v>63</v>
       </c>
       <c r="E59" s="30"/>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="14"/>
       <c r="D60" s="29" t="s">
         <v>64</v>
       </c>
       <c r="E60" s="30"/>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="14"/>
       <c r="D61" s="29" t="s">
         <v>65</v>
       </c>
       <c r="E61" s="30"/>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="14"/>
       <c r="D62" s="29" t="s">
         <v>66</v>
       </c>
       <c r="E62" s="30"/>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="14"/>
       <c r="B63" s="12"/>
       <c r="C63" s="12"/>
@@ -1675,38 +1833,38 @@
       <c r="E63" s="31"/>
       <c r="F63" s="21"/>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="14"/>
       <c r="D64" s="29" t="s">
         <v>68</v>
       </c>
       <c r="E64" s="30"/>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D65" s="29" t="s">
         <v>69</v>
       </c>
       <c r="E65" s="30"/>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D66" s="29" t="s">
         <v>70</v>
       </c>
       <c r="E66" s="30"/>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D67" s="29" t="s">
         <v>71</v>
       </c>
       <c r="E67" s="30"/>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D68" s="29" t="s">
         <v>72</v>
       </c>
       <c r="E68" s="30"/>
     </row>
-    <row r="69" spans="1:6" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="14"/>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
@@ -1716,7 +1874,7 @@
       <c r="E69" s="7"/>
       <c r="F69" s="18"/>
     </row>
-    <row r="70" spans="1:6" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="16"/>
       <c r="B70" s="11"/>
       <c r="C70" s="11"/>
@@ -1726,7 +1884,7 @@
       <c r="E70" s="27"/>
       <c r="F70" s="19"/>
     </row>
-    <row r="71" spans="1:6" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="28"/>
       <c r="B71" s="12"/>
       <c r="C71" s="12"/>
@@ -1736,7 +1894,7 @@
       <c r="E71" s="31"/>
       <c r="F71" s="21"/>
     </row>
-    <row r="72" spans="1:6" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="15"/>
       <c r="B72" s="10"/>
       <c r="C72" s="33"/>
@@ -1746,7 +1904,7 @@
       <c r="E72" s="30"/>
       <c r="F72" s="20"/>
     </row>
-    <row r="73" spans="1:6" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="15"/>
       <c r="B73" s="10"/>
       <c r="C73" s="10"/>
@@ -1756,7 +1914,7 @@
       <c r="E73" s="30"/>
       <c r="F73" s="20"/>
     </row>
-    <row r="74" spans="1:6" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="15"/>
       <c r="B74" s="10"/>
       <c r="C74" s="10"/>
@@ -1766,7 +1924,7 @@
       <c r="E74" s="30"/>
       <c r="F74" s="22"/>
     </row>
-    <row r="75" spans="1:6" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="15"/>
       <c r="B75" s="10"/>
       <c r="C75" s="10"/>
@@ -1776,13 +1934,13 @@
       <c r="E75" s="30"/>
       <c r="F75" s="20"/>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D76" s="29" t="s">
         <v>80</v>
       </c>
       <c r="E76" s="30"/>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="16"/>
       <c r="B77" s="11"/>
       <c r="C77" s="11"/>
@@ -1792,130 +1950,130 @@
       <c r="E77" s="27"/>
       <c r="F77" s="19"/>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D78" s="29" t="s">
         <v>82</v>
       </c>
       <c r="E78" s="30"/>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D79" s="29" t="s">
         <v>83</v>
       </c>
       <c r="E79" s="30"/>
     </row>
-    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D80" s="29" t="s">
         <v>84</v>
       </c>
       <c r="E80" s="30"/>
     </row>
-    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D81" s="29" t="s">
         <v>85</v>
       </c>
       <c r="E81" s="30"/>
     </row>
-    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D82" s="29" t="s">
         <v>86</v>
       </c>
       <c r="E82" s="30"/>
     </row>
-    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D83" s="29" t="s">
         <v>87</v>
       </c>
       <c r="E83" s="30"/>
     </row>
-    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D84" s="29" t="s">
         <v>88</v>
       </c>
       <c r="E84" s="30"/>
     </row>
-    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D85" s="29" t="s">
         <v>89</v>
       </c>
       <c r="E85" s="30"/>
     </row>
-    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D86" s="29" t="s">
         <v>90</v>
       </c>
       <c r="E86" s="30"/>
     </row>
-    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D87" s="29" t="s">
         <v>91</v>
       </c>
       <c r="E87" s="30"/>
     </row>
-    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D88" s="29" t="s">
         <v>92</v>
       </c>
       <c r="E88" s="30"/>
     </row>
-    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D89" s="29" t="s">
         <v>93</v>
       </c>
       <c r="E89" s="30"/>
     </row>
-    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D90" s="29" t="s">
         <v>94</v>
       </c>
       <c r="E90" s="30"/>
     </row>
-    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D91" s="29" t="s">
         <v>95</v>
       </c>
       <c r="E91" s="30"/>
     </row>
-    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D92" s="29" t="s">
         <v>96</v>
       </c>
       <c r="E92" s="30"/>
     </row>
-    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D93" s="29" t="s">
         <v>97</v>
       </c>
       <c r="E93" s="30"/>
     </row>
-    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="14"/>
       <c r="D94" s="29" t="s">
         <v>98</v>
       </c>
       <c r="E94" s="30"/>
     </row>
-    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D95" s="29" t="s">
         <v>99</v>
       </c>
       <c r="E95" s="30"/>
     </row>
-    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="14"/>
       <c r="D96" s="29" t="s">
         <v>100</v>
       </c>
       <c r="E96" s="30"/>
     </row>
-    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="14"/>
       <c r="D97" s="29" t="s">
         <v>101</v>
       </c>
       <c r="E97" s="30"/>
     </row>
-    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="16"/>
       <c r="B98" s="11"/>
       <c r="C98" s="11"/>
@@ -1925,7 +2083,7 @@
       <c r="E98" s="27"/>
       <c r="F98" s="19"/>
     </row>
-    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="16"/>
       <c r="B99" s="11"/>
       <c r="C99" s="11"/>
@@ -1935,19 +2093,19 @@
       <c r="E99" s="27"/>
       <c r="F99" s="19"/>
     </row>
-    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D100" s="29" t="s">
         <v>104</v>
       </c>
       <c r="E100" s="32"/>
     </row>
-    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D101" s="29" t="s">
         <v>105</v>
       </c>
       <c r="E101" s="32"/>
     </row>
-    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="28"/>
       <c r="B102" s="12"/>
       <c r="C102" s="12"/>
@@ -1957,70 +2115,70 @@
       <c r="E102" s="31"/>
       <c r="F102" s="21"/>
     </row>
-    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D103" s="29" t="s">
         <v>107</v>
       </c>
       <c r="E103" s="30"/>
     </row>
-    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D104" s="29" t="s">
         <v>108</v>
       </c>
       <c r="E104" s="30"/>
     </row>
-    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D105" s="29" t="s">
         <v>109</v>
       </c>
       <c r="E105" s="32"/>
       <c r="F105" s="22"/>
     </row>
-    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D106" s="29" t="s">
         <v>110</v>
       </c>
       <c r="E106" s="30"/>
     </row>
-    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D107" s="29" t="s">
         <v>111</v>
       </c>
       <c r="E107" s="32"/>
       <c r="F107" s="22"/>
     </row>
-    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D108" s="29" t="s">
         <v>112</v>
       </c>
       <c r="E108" s="30"/>
     </row>
-    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D109" s="29" t="s">
         <v>113</v>
       </c>
       <c r="E109" s="30"/>
     </row>
-    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D110" s="29" t="s">
         <v>114</v>
       </c>
       <c r="E110" s="30"/>
     </row>
-    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D111" s="29" t="s">
         <v>115</v>
       </c>
       <c r="E111" s="30"/>
     </row>
-    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D112" s="29" t="s">
         <v>116</v>
       </c>
       <c r="E112" s="30"/>
       <c r="G112" s="22"/>
     </row>
-    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="23"/>
       <c r="B113" s="24"/>
       <c r="C113" s="24"/>
@@ -2030,19 +2188,19 @@
       <c r="E113" s="32"/>
       <c r="F113" s="22"/>
     </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D114" s="29" t="s">
         <v>118</v>
       </c>
       <c r="E114" s="30"/>
     </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D115" s="29" t="s">
         <v>119</v>
       </c>
       <c r="E115" s="30"/>
     </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="16"/>
       <c r="B116" s="11"/>
       <c r="C116" s="11"/>
@@ -2052,161 +2210,84 @@
       <c r="E116" s="27"/>
       <c r="F116" s="19"/>
     </row>
-    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D117" s="29" t="s">
         <v>121</v>
       </c>
       <c r="E117" s="30"/>
     </row>
-    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D118" s="29" t="s">
         <v>122</v>
       </c>
       <c r="E118" s="30"/>
     </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D119" s="29" t="s">
         <v>123</v>
       </c>
       <c r="E119" s="30"/>
     </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D120" s="29" t="s">
         <v>124</v>
       </c>
       <c r="E120" s="30"/>
     </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D121" s="29" t="s">
         <v>125</v>
       </c>
       <c r="E121" s="30"/>
     </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D122" s="29" t="s">
         <v>126</v>
       </c>
       <c r="E122" s="30"/>
     </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D123" s="29" t="s">
         <v>127</v>
       </c>
       <c r="E123" s="32"/>
     </row>
-    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D124" s="29" t="s">
         <v>128</v>
       </c>
       <c r="E124" s="30"/>
     </row>
-    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D125" s="29" t="s">
         <v>129</v>
       </c>
       <c r="E125" s="30"/>
     </row>
-    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D126" s="29" t="s">
         <v>130</v>
       </c>
       <c r="E126" s="30"/>
     </row>
-    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D127" s="29" t="s">
         <v>131</v>
       </c>
       <c r="E127" s="30"/>
     </row>
-    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D128" s="29" t="s">
         <v>132</v>
       </c>
       <c r="E128" s="30"/>
     </row>
-    <row r="129" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="130" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="131" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="132" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="133" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="134" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="135" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="136" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="137" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="138" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="139" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="140" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="141" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="142" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="143" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="144" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="145" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="146" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="147" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="148" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="149" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="150" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="151" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="152" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="153" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="154" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="155" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="156" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="157" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="158" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="159" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="160" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="161" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="162" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="163" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="164" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="165" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="166" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="167" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="168" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="169" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="170" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="171" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="172" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="173" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="174" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="175" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="176" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="177" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="178" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="179" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="180" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="181" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="182" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="183" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="184" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="185" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="186" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="187" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="188" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="189" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="190" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="191" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="192" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="193" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="194" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="195" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="196" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="197" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="198" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="199" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="200" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="201" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="202" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A1:G202">
     <filterColumn colId="0">
-      <filters>
-        <filter val="alpha-3"/>
+      <filters blank="1">
+        <filter val="alpha-4"/>
       </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Separated the font specifications into two lines, since the w3c markup checker tool complained about illegal character in href attribute for the font link
</commit_message>
<xml_diff>
--- a/doc/bugs.xlsx
+++ b/doc/bugs.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="166">
   <si>
     <t>Datum rapporterat</t>
   </si>
@@ -434,9 +434,6 @@
   </si>
   <si>
     <t>Någon form av byggmekanism så att endast de filer som är relevanta för hemsidan kopieras till en deploymentkatalog</t>
-  </si>
-  <si>
-    <t>Lös problemet med att rubrikerna syns i index.html när man surfar in på sidan</t>
   </si>
   <si>
     <t>Registrera sajten hos Google</t>
@@ -518,9 +515,6 @@
     <t>Kolla om det är flera meta-taggar som behövs. Sajten heter www.metatags.org.</t>
   </si>
   <si>
-    <t>Lägg till musiklyssning och fotografering som personliga intressen.</t>
-  </si>
-  <si>
     <t>Byt bakgrundsmönster till något trevligare, mer levande.</t>
   </si>
   <si>
@@ -536,7 +530,47 @@
     <t>Nu skall SEO-arbetet påbörjas på riktigt.</t>
   </si>
   <si>
-    <t>Går det att få till en högersida i Google som visar bara kontaktinformationen?</t>
+    <t>Lägg till musiklyssning och fotografering som personliga intressen. Ge exempel på några av mina favoritartister.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lös problemet med att rubrikerna syns i index.html när man surfar in på sidan. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ärendet lämnas utan åtgärd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Går det att få till en högersida i Googles sökresultat som visar bara kontaktinformationen?</t>
+  </si>
+  <si>
+    <t>Gör col-sm6 av brödtexten i index.html så blir den likadan som resten av sajten.</t>
+  </si>
+  <si>
+    <t>Kör w3c markup analyzer tool på html-filerna</t>
+  </si>
+  <si>
+    <t>Kör w3c markup analyzer tool på css-filen</t>
+  </si>
+  <si>
+    <t>Fontspecifikationerna måste anges en och en, inte Lobster|Play - w3c markup tool klagar</t>
   </si>
 </sst>
 </file>
@@ -1027,8 +1061,8 @@
   <dimension ref="A1:G128"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,12 +1114,12 @@
         <v>7</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B3" s="9">
         <v>43202</v>
@@ -1115,7 +1149,7 @@
         <v>7</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1153,7 +1187,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1173,17 +1207,19 @@
         <v>8</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B8" s="9">
         <v>43202</v>
       </c>
-      <c r="C8" s="9"/>
+      <c r="C8" s="9">
+        <v>41745</v>
+      </c>
       <c r="D8" s="29" t="s">
         <v>12</v>
       </c>
@@ -1191,7 +1227,7 @@
         <v>7</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1211,12 +1247,12 @@
         <v>7</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B10" s="9">
         <v>43202</v>
@@ -1229,7 +1265,7 @@
         <v>6</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1249,7 +1285,7 @@
         <v>6</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -1269,13 +1305,13 @@
         <v>7</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B13" s="9">
         <v>43202</v>
@@ -1290,7 +1326,7 @@
         <v>6</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1310,7 +1346,7 @@
         <v>6</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1330,12 +1366,12 @@
         <v>8</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B16" s="9">
         <v>43202</v>
@@ -1350,7 +1386,7 @@
         <v>8</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -1370,7 +1406,7 @@
         <v>6</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -1390,12 +1426,12 @@
         <v>7</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B19" s="9">
         <v>43205</v>
@@ -1408,7 +1444,7 @@
         <v>7</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -1428,12 +1464,12 @@
         <v>7</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B21" s="9">
         <v>43205</v>
@@ -1446,12 +1482,12 @@
         <v>6</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B22" s="9">
         <v>43205</v>
@@ -1464,12 +1500,12 @@
         <v>6</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B23" s="9">
         <v>43205</v>
@@ -1482,12 +1518,12 @@
         <v>7</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B24" s="9">
         <v>43205</v>
@@ -1498,12 +1534,12 @@
       </c>
       <c r="E24" s="30"/>
       <c r="F24" s="20" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B25" s="9">
         <v>43205</v>
@@ -1515,12 +1551,12 @@
         <v>8</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B26" s="9">
         <v>43205</v>
@@ -1533,12 +1569,12 @@
         <v>6</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B27" s="9">
         <v>43205</v>
@@ -1550,12 +1586,12 @@
         <v>7</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B28" s="9">
         <v>43205</v>
@@ -1571,37 +1607,81 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
+      <c r="A29" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" s="10">
+        <v>43206</v>
+      </c>
       <c r="D29" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="E29" s="30"/>
+      <c r="E29" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
+      <c r="A30" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B30" s="10">
+        <v>43206</v>
+      </c>
       <c r="D30" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="E30" s="30"/>
+      <c r="E30" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="11"/>
+      <c r="A31" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B31" s="10">
+        <v>43206</v>
+      </c>
       <c r="C31" s="11"/>
       <c r="D31" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="E31" s="27"/>
-      <c r="F31" s="19"/>
+      <c r="E31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B32" s="10">
+        <v>43206</v>
+      </c>
+      <c r="C32" s="10">
+        <v>43206</v>
+      </c>
       <c r="D32" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="E32" s="30"/>
+      <c r="E32" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
+      <c r="A33" s="14" t="s">
+        <v>140</v>
+      </c>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
       <c r="D33" s="29" t="s">
@@ -1611,6 +1691,9 @@
       <c r="F33" s="21"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>140</v>
+      </c>
       <c r="D34" s="29" t="s">
         <v>38</v>
       </c>
@@ -2285,7 +2368,7 @@
   </sheetData>
   <autoFilter ref="A1:G202">
     <filterColumn colId="0">
-      <filters blank="1">
+      <filters>
         <filter val="alpha-4"/>
       </filters>
     </filterColumn>

</xml_diff>

<commit_message>
Added bing site owner verification xml file
</commit_message>
<xml_diff>
--- a/doc/bugs.xlsx
+++ b/doc/bugs.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="167">
   <si>
     <t>Datum rapporterat</t>
   </si>
@@ -571,6 +571,9 @@
   </si>
   <si>
     <t>Fontspecifikationerna måste anges en och en, inte Lobster|Play - w3c markup tool klagar</t>
+  </si>
+  <si>
+    <t>Hitta en liten emailikon</t>
   </si>
 </sst>
 </file>
@@ -1060,9 +1063,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1682,13 +1685,19 @@
       <c r="A33" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="B33" s="12"/>
+      <c r="B33" s="12">
+        <v>43207</v>
+      </c>
       <c r="C33" s="12"/>
       <c r="D33" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="E33" s="31"/>
-      <c r="F33" s="21"/>
+      <c r="E33" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" s="21" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
@@ -1700,7 +1709,9 @@
       <c r="E34" s="30"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
+      <c r="A35" s="14" t="s">
+        <v>140</v>
+      </c>
       <c r="C35" s="9"/>
       <c r="D35" s="29" t="s">
         <v>39</v>
@@ -1708,6 +1719,9 @@
       <c r="E35" s="30"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>140</v>
+      </c>
       <c r="C36" s="9"/>
       <c r="D36" s="29" t="s">
         <v>40</v>
@@ -1715,6 +1729,9 @@
       <c r="E36" s="30"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>140</v>
+      </c>
       <c r="C37" s="9"/>
       <c r="D37" s="29" t="s">
         <v>41</v>
@@ -1722,7 +1739,9 @@
       <c r="E37" s="30"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
+      <c r="A38" s="14" t="s">
+        <v>140</v>
+      </c>
       <c r="C38" s="9"/>
       <c r="D38" s="29" t="s">
         <v>42</v>
@@ -1730,6 +1749,9 @@
       <c r="E38" s="30"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>140</v>
+      </c>
       <c r="C39" s="9"/>
       <c r="D39" s="29" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
obfuscated the protocols "tel:" and "mailto:" to create complete confusion
</commit_message>
<xml_diff>
--- a/doc/bugs.xlsx
+++ b/doc/bugs.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="169">
   <si>
     <t>Datum rapporterat</t>
   </si>
@@ -574,6 +574,12 @@
   </si>
   <si>
     <t>Hitta en liten emailikon</t>
+  </si>
+  <si>
+    <t>Försök koda om mailto-länken så att även ordet "mailto:" kodas i index.html</t>
+  </si>
+  <si>
+    <t>Försök koda om tel-länken pss som #33</t>
   </si>
 </sst>
 </file>
@@ -1063,9 +1069,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1703,20 +1709,41 @@
       <c r="A34" s="14" t="s">
         <v>140</v>
       </c>
+      <c r="B34" s="12">
+        <v>43207</v>
+      </c>
+      <c r="C34" s="12">
+        <v>43207</v>
+      </c>
       <c r="D34" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="E34" s="30"/>
+      <c r="E34" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="C35" s="9"/>
+      <c r="B35" s="12">
+        <v>43207</v>
+      </c>
+      <c r="C35" s="12">
+        <v>43207</v>
+      </c>
       <c r="D35" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="E35" s="30"/>
+      <c r="E35" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">

</xml_diff>

<commit_message>
obfuscated my cell phone number
</commit_message>
<xml_diff>
--- a/doc/bugs.xlsx
+++ b/doc/bugs.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="170">
   <si>
     <t>Datum rapporterat</t>
   </si>
@@ -509,9 +509,6 @@
 Kod för Google Analytics implementerad på annat, nytt sätt.</t>
   </si>
   <si>
-    <t>Varje sida skall ha åtminstone en h2-rubrik</t>
-  </si>
-  <si>
     <t>Kolla om det är flera meta-taggar som behövs. Sajten heter www.metatags.org.</t>
   </si>
   <si>
@@ -580,6 +577,12 @@
   </si>
   <si>
     <t>Försök koda om tel-länken pss som #33</t>
+  </si>
+  <si>
+    <t>Varje sida skall ha åtminstone en h1 och h2-rubrik</t>
+  </si>
+  <si>
+    <t>"Jag finns även på" ovanför bilden på LinkedIn</t>
   </si>
 </sst>
 </file>
@@ -1069,9 +1072,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,7 +1239,7 @@
         <v>7</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1266,7 +1269,9 @@
       <c r="B10" s="9">
         <v>43202</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="9">
+        <v>41746</v>
+      </c>
       <c r="D10" s="29" t="s">
         <v>14</v>
       </c>
@@ -1473,7 +1478,7 @@
         <v>7</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1491,7 +1496,7 @@
         <v>6</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1509,7 +1514,7 @@
         <v>6</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1527,7 +1532,7 @@
         <v>7</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1541,9 +1546,11 @@
       <c r="D24" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="30"/>
+      <c r="E24" s="30" t="s">
+        <v>6</v>
+      </c>
       <c r="F24" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1560,7 +1567,7 @@
         <v>8</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1578,7 +1585,7 @@
         <v>6</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1595,7 +1602,7 @@
         <v>7</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1612,7 +1619,7 @@
         <v>6</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1629,7 +1636,7 @@
         <v>6</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1646,7 +1653,7 @@
         <v>7</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1664,7 +1671,7 @@
         <v>7</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1684,7 +1691,7 @@
         <v>7</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1702,7 +1709,7 @@
         <v>6</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1722,7 +1729,7 @@
         <v>7</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1742,18 +1749,28 @@
         <v>7</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="C36" s="9"/>
+      <c r="B36" s="10">
+        <v>43212</v>
+      </c>
+      <c r="C36" s="10">
+        <v>43212</v>
+      </c>
       <c r="D36" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="E36" s="30"/>
+      <c r="E36" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">

</xml_diff>